<commit_message>
#2 updated mint and maxt columns to mintp and maxtp
</commit_message>
<xml_diff>
--- a/data/Met_Eireann/ucc.xlsx
+++ b/data/Met_Eireann/ucc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\IrishClimateApp\data\Met_Eireann\arch\UCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\IrishClimateApp\data\Met_Eireann\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DC1257B6-711B-4F31-92A0-A92E9C09D515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B25D97C-041A-46BF-94E0-873685C8B545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dly7404" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -920,14 +920,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -970,7 +983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
#2 ordering rows in master file by county and station
</commit_message>
<xml_diff>
--- a/data/Met_Eireann/ucc.xlsx
+++ b/data/Met_Eireann/ucc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\IrishClimateApp\data\Met_Eireann\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B25D97C-041A-46BF-94E0-873685C8B545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73D4DDB-3FBC-4469-865A-D53FB267A456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,12 +41,6 @@
     <t>rain: -   Precipitation Amount (mm)</t>
   </si>
   <si>
-    <t>maxt: -   Maximum Temperature (C)</t>
-  </si>
-  <si>
-    <t>mint: -   Minimum Temperature (C)</t>
-  </si>
-  <si>
     <t>gmin: -   09utc Grass Minimum Temperature (C)</t>
   </si>
   <si>
@@ -65,12 +59,6 @@
     <t>rain</t>
   </si>
   <si>
-    <t>maxt</t>
-  </si>
-  <si>
-    <t>mint</t>
-  </si>
-  <si>
     <t>gmin</t>
   </si>
   <si>
@@ -81,6 +69,18 @@
   </si>
   <si>
     <t>county</t>
+  </si>
+  <si>
+    <t>mintp</t>
+  </si>
+  <si>
+    <t>maxtp</t>
+  </si>
+  <si>
+    <t>mintp: -   Minimum Temperature (C)</t>
+  </si>
+  <si>
+    <t>maxtp: -   Maximum Temperature (C)</t>
   </si>
 </sst>
 </file>
@@ -924,7 +924,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,46 +935,46 @@
     <col min="4" max="4" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -987,7 +987,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,27 +1022,27 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>